<commit_message>
Propuesta de socios comerciales
En las bases de importaciones y exportaciones por aduana, se encuentra un hoja de que llama "PROPUESTA"
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/Datos/Importaciones-por-aduanas-en-Santa-Fe-segun-destino-2018-2024.xlsx
+++ b/Archivos de trabajo/Datos/Importaciones-por-aduanas-en-Santa-Fe-segun-destino-2018-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcorvalan\Desktop\Trabajo\Paper\Paper-ITCRM.SF\Archivos de trabajo\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D45482-5995-43ED-A76C-E9F8F7F7FD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED534AD-C32D-4E9C-A5BB-A36B8F9FA36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,11 @@
     <sheet name="ACUMULADO" sheetId="4" r:id="rId2"/>
     <sheet name="ANUAL" sheetId="6" r:id="rId3"/>
     <sheet name="SOCIOS" sheetId="7" r:id="rId4"/>
+    <sheet name="PROPUESTA" sheetId="8" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PROPUESTA!$B$2:$D$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="39">
   <si>
     <t>Título</t>
   </si>
@@ -146,6 +150,15 @@
   <si>
     <t>Nigeria</t>
   </si>
+  <si>
+    <t xml:space="preserve">País </t>
+  </si>
+  <si>
+    <t>Cantidad de veces mayor al 2%</t>
+  </si>
+  <si>
+    <t>Participación promedio (2018-2024)</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +219,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -245,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -677,6 +696,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -684,7 +790,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,6 +895,31 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1075,10 +1206,10 @@
   <dimension ref="B1:AG160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8297,23 +8428,23 @@
       <c r="B65" s="14">
         <v>2023.01</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="36">
         <v>232000000</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="32">
         <v>12200000</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="21">
         <v>66800000</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="21">
         <v>26700000</v>
       </c>
       <c r="G65" s="21" t="str">
         <f>IF(AND(ACUMULADO!G65&lt;&gt;"",ACUMULADO!G64&lt;&gt;""),ACUMULADO!G65-ACUMULADO!G64,"")</f>
         <v/>
       </c>
-      <c r="H65">
+      <c r="H65" s="21">
         <v>42800000</v>
       </c>
       <c r="I65" s="21" t="str">
@@ -8324,10 +8455,10 @@
         <f>IF(AND(ACUMULADO!J65&lt;&gt;"",ACUMULADO!J64&lt;&gt;""),ACUMULADO!J65-ACUMULADO!J64,"")</f>
         <v/>
       </c>
-      <c r="K65">
+      <c r="K65" s="21">
         <v>7100000</v>
       </c>
-      <c r="L65">
+      <c r="L65" s="21">
         <v>8700000</v>
       </c>
       <c r="M65" s="21" t="str">
@@ -8338,7 +8469,7 @@
         <f>IF(AND(ACUMULADO!N65&lt;&gt;"",ACUMULADO!N64&lt;&gt;""),ACUMULADO!N65-ACUMULADO!N64,"")</f>
         <v/>
       </c>
-      <c r="O65">
+      <c r="O65" s="21">
         <v>2900000</v>
       </c>
       <c r="P65" s="21" t="str">
@@ -8361,7 +8492,7 @@
         <f>IF(AND(ACUMULADO!T65&lt;&gt;"",ACUMULADO!T64&lt;&gt;""),ACUMULADO!T65-ACUMULADO!T64,"")</f>
         <v/>
       </c>
-      <c r="U65">
+      <c r="U65" s="21">
         <v>3400000</v>
       </c>
       <c r="V65" s="21" t="str">
@@ -8380,7 +8511,7 @@
         <f>IF(AND(ACUMULADO!Y65&lt;&gt;"",ACUMULADO!Y64&lt;&gt;""),ACUMULADO!Y65-ACUMULADO!Y64,"")</f>
         <v/>
       </c>
-      <c r="Z65">
+      <c r="Z65" s="21">
         <v>40500000</v>
       </c>
       <c r="AA65" s="21" t="str">
@@ -8407,7 +8538,7 @@
         <f>IF(AND(ACUMULADO!AF65&lt;&gt;"",ACUMULADO!AF64&lt;&gt;""),ACUMULADO!AF65-ACUMULADO!AF64,"")</f>
         <v/>
       </c>
-      <c r="AG65">
+      <c r="AG65" s="22">
         <v>16600000.000000002</v>
       </c>
     </row>
@@ -18630,10 +18761,10 @@
   <dimension ref="B1:AG160"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I105" sqref="I105"/>
+      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33581,7 +33712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7097AD37-8A90-440E-B5A1-5B878B168DAE}">
   <dimension ref="B1:U22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -34612,7 +34743,7 @@
   <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35788,4 +35919,164 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A5E4F2-7EA7-436F-882D-3F0FA582FEB9}">
+  <dimension ref="B1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="56">
+        <v>7</v>
+      </c>
+      <c r="D3" s="57">
+        <v>0.37989619138322012</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="56">
+        <v>7</v>
+      </c>
+      <c r="D4" s="57">
+        <v>0.23707536285978717</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="56">
+        <v>7</v>
+      </c>
+      <c r="D5" s="57">
+        <v>0.10694015153013858</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="56">
+        <v>7</v>
+      </c>
+      <c r="D6" s="57">
+        <v>0.10039830576767396</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="56">
+        <v>7</v>
+      </c>
+      <c r="D7" s="57">
+        <v>7.4854620049196213E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="56">
+        <v>2</v>
+      </c>
+      <c r="D8" s="57">
+        <v>4.1431724684943438E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="56">
+        <v>2</v>
+      </c>
+      <c r="D9" s="57">
+        <v>2.7653776467242614E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="56">
+        <v>1</v>
+      </c>
+      <c r="D10" s="57">
+        <v>2.1746655668916301E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="56">
+        <v>2</v>
+      </c>
+      <c r="D11" s="57">
+        <v>1.7604905554066096E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="56">
+        <v>1</v>
+      </c>
+      <c r="D12" s="57">
+        <v>1.6262331661128584E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="59">
+        <v>1</v>
+      </c>
+      <c r="D13" s="60">
+        <v>1.4477325303826753E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:D13" xr:uid="{71A5E4F2-7EA7-436F-882D-3F0FA582FEB9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D13">
+      <sortCondition descending="1" ref="D2:D13"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>